<commit_message>
Criação do documento de Iteração_ E1 atualização da lista de itens correçaão e atualização do plano de projeto
</commit_message>
<xml_diff>
--- a/planejamento/RT_Lista_Itens.xlsx
+++ b/planejamento/RT_Lista_Itens.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="45">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -118,9 +118,21 @@
     <t>Alteração Plano de Projeto  </t>
   </si>
   <si>
+    <t>Iniciado</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
     <t>Criação do  Plano de Interação  E1</t>
   </si>
   <si>
+    <t>Atualizar Lista de Riscos </t>
+  </si>
+  <si>
+    <t>1/2 de hora</t>
+  </si>
+  <si>
     <t>Alteração Lista de Itens</t>
   </si>
   <si>
@@ -131,6 +143,9 @@
   </si>
   <si>
     <t>Implementação dos Requisitos de Cadastro</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
   </si>
   <si>
     <t>Implementação dos Requisitos de Entrega</t>
@@ -250,7 +265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -301,6 +316,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -384,24 +403,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="B17:G25"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.9744897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.2295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.2091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.6326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.9336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.0459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.3520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.4438775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="32.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.25510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,83 +864,239 @@
       <c r="A18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="I18" s="13"/>
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="H18" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="I19" s="13"/>
+      <c r="E19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="I20" s="13"/>
+      <c r="F20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="I21" s="0"/>
+        <v>38</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="I22" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="H22" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="I23" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="I24" s="13"/>
+        <v>41</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="14"/>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="I25" s="13"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>43</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A14:I15"/>
@@ -944,12 +1119,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B17:G25 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.25510204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -970,12 +1145,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B17:G25 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.25510204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Correções e alterações dos artefatos
</commit_message>
<xml_diff>
--- a/planejamento/RT_Lista_Itens.xlsx
+++ b/planejamento/RT_Lista_Itens.xlsx
@@ -406,21 +406,20 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.9336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.0459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.3520408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.1530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.4438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="32.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.25510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.6836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.1938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.2244897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,7 +1043,9 @@
       <c r="G24" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="H24" s="13"/>
+      <c r="H24" s="13" t="n">
+        <v>2</v>
+      </c>
       <c r="I24" s="14"/>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,7 +1059,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>34</v>
@@ -1069,7 +1070,9 @@
       <c r="G25" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="H25" s="13"/>
+      <c r="H25" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="I25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,6 +1096,9 @@
       </c>
       <c r="G26" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I26" s="14"/>
     </row>
@@ -1123,9 +1129,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.25510204081633"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1149,9 +1152,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.25510204081633"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Correções e elaboração do plano de iteração
</commit_message>
<xml_diff>
--- a/planejamento/RT_Lista_Itens.xlsx
+++ b/planejamento/RT_Lista_Itens.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -94,6 +94,12 @@
     <t>Definir a arquitetura preliminar</t>
   </si>
   <si>
+    <t>Elaborar Plano de Iteração</t>
+  </si>
+  <si>
+    <t>Projeto SchoolDrive, Orientação em aulas</t>
+  </si>
+  <si>
     <t>Definir a lista de riscos</t>
   </si>
   <si>
@@ -118,21 +124,12 @@
     <t>Alteração Plano de Projeto  </t>
   </si>
   <si>
-    <t>Iniciado</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
     <t>Criação do  Plano de Interação  E1</t>
   </si>
   <si>
     <t>Atualizar Lista de Riscos </t>
   </si>
   <si>
-    <t>1/2 de hora</t>
-  </si>
-  <si>
     <t>Alteração Lista de Itens</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
   </si>
   <si>
     <t>Implementação dos Requisitos de Cadastro</t>
-  </si>
-  <si>
-    <t>Em andamento</t>
   </si>
   <si>
     <t>Implementação dos Requisitos de Entrega</t>
@@ -265,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -286,16 +280,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -315,6 +309,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,23 +401,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.6836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.1938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.2244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.8265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.3367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.1938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4897959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6632653061224"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="35.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.86734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,7 +450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -480,7 +479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -509,7 +508,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -538,7 +537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -567,7 +566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -578,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -596,7 +595,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -606,7 +605,7 @@
       <c r="C7" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -625,7 +624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -635,26 +634,26 @@
       <c r="C8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
@@ -662,84 +661,86 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="D10" s="0" t="s">
+      <c r="I10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G11" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H11" s="0"/>
       <c r="I11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
@@ -747,69 +748,85 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H12" s="0"/>
+        <v>5</v>
+      </c>
+      <c r="H12" s="6"/>
       <c r="I12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>30</v>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>17</v>
+      <c r="D13" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H13" s="1" t="n">
+      <c r="H13" s="6"/>
+      <c r="I13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
+      <c r="D14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
+      <c r="A15" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -820,292 +837,174 @@
       <c r="I15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I17" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" s="12" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="6" t="s">
+    <row r="18" s="12" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="H18" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="I18" s="14"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="H19" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="I19" s="14"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="13" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="I20" s="14"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="I21" s="14"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="H22" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="I22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+      <c r="B24" s="6"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="H23" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="I23" s="14"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="B25" s="6"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="13" t="n">
-        <v>6</v>
-      </c>
-      <c r="D24" s="13" t="s">
+      <c r="B26" s="6"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="H24" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="I24" s="14"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="13" t="n">
-        <v>8</v>
-      </c>
-      <c r="H25" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" s="14"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A14:I15"/>
+    <mergeCell ref="A15:I16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1129,6 +1028,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.86734693877551"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1152,6 +1054,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.86734693877551"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Correções e Atualizações dos artefatos
</commit_message>
<xml_diff>
--- a/planejamento/RT_Lista_Itens.xlsx
+++ b/planejamento/RT_Lista_Itens.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Itens de Trabalho" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,11 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -109,10 +114,10 @@
     <t>Implementar os protótipos de GUI</t>
   </si>
   <si>
+    <t>Preparar a apresentação</t>
+  </si>
+  <si>
     <t>Não Iniciado</t>
-  </si>
-  <si>
-    <t>Preparar a apresentação</t>
   </si>
   <si>
     <t>Configuração da IDE + Criação do projeto</t>
@@ -333,21 +338,21 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.2397959183674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.4489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.2040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.2602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.9744897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="32.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.25510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,7 +656,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
@@ -680,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
@@ -691,14 +696,16 @@
       <c r="G12" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="6" t="n">
+        <v>5</v>
+      </c>
       <c r="I12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -707,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
@@ -761,6 +768,16 @@
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+      <c r="F16" s="0"/>
+      <c r="G16" s="0"/>
+      <c r="H16" s="0"/>
+      <c r="I16" s="0"/>
     </row>
     <row r="18" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0"/>
@@ -797,7 +814,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.25510204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -823,7 +840,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.25510204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Criação do Plano de iteração E1
</commit_message>
<xml_diff>
--- a/planejamento/RT_Lista_Itens.xlsx
+++ b/planejamento/RT_Lista_Itens.xlsx
@@ -337,21 +337,21 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.9030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.9540816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.5867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.3367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.3316326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.9132653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.6224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="39.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.9744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.0561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.9744897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="38.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.48469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +568,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>12</v>
@@ -812,6 +812,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -835,6 +838,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Atualizações e correções de artefatos
</commit_message>
<xml_diff>
--- a/planejamento/RT_Lista_Itens.xlsx
+++ b/planejamento/RT_Lista_Itens.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="47">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -121,6 +121,48 @@
   </si>
   <si>
     <t>Configuração da IDE + Criação do projeto</t>
+  </si>
+  <si>
+    <t>Fase de Elaboração E1</t>
+  </si>
+  <si>
+    <t>Alteração Plano de Projeto  </t>
+  </si>
+  <si>
+    <t>Iniciado</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>Criação do  Plano de Interação  E1</t>
+  </si>
+  <si>
+    <t>Atualizar Lista de Riscos </t>
+  </si>
+  <si>
+    <t>1/2 de hora</t>
+  </si>
+  <si>
+    <t>Alteração Lista de Itens</t>
+  </si>
+  <si>
+    <t>Refinamento Requisitos de Cadastro</t>
+  </si>
+  <si>
+    <t>Refinamento Requisito de Entrega </t>
+  </si>
+  <si>
+    <t>Implementação dos Requisitos de Cadastro</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Implementação dos Requisitos de Entrega</t>
+  </si>
+  <si>
+    <t>Modelagem de analise e projeto</t>
   </si>
 </sst>
 </file>
@@ -160,7 +202,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,12 +217,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -192,6 +240,13 @@
       <left style="thin"/>
       <right style="thin"/>
       <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -221,7 +276,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,8 +309,36 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -335,23 +418,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.2091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.9744897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.0561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.9744897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="38.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.984693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.3520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="11.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.2908163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.3520408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="37.0255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.17857142857143"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,38 +841,317 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="D15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
-      <c r="G15" s="0"/>
-      <c r="H15" s="0"/>
-      <c r="I15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="D16" s="0"/>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
-      <c r="G16" s="0"/>
-      <c r="H16" s="0"/>
-      <c r="I16" s="0"/>
-    </row>
-    <row r="18" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="D18" s="0"/>
-      <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
-      <c r="G18" s="0"/>
-      <c r="H18" s="0"/>
-      <c r="I18" s="0"/>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" s="12" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H24" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="H25" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="14" t="n">
+        <v>8</v>
+      </c>
+      <c r="H26" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" s="15"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:I16"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -813,7 +1175,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.17857142857143"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -839,7 +1201,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.17857142857143"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>